<commit_message>
Abstract out a generic assertion
This is a test to see how it looks with generic assertions, inheritance, and multiple type bindings.
</commit_message>
<xml_diff>
--- a/anvil/excel/anvil.xlsx
+++ b/anvil/excel/anvil.xlsx
@@ -9,18 +9,22 @@
   <sheets>
     <sheet name="Thing" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="AccessControlledRecord" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Study" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Sample" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Subject" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Participant" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Any" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Study" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Sample" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="SubjectAssertion" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="ConditionAssertion" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="AccessPolicy" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="BiospecimenCollection" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Aliquot" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="Measurement" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="Procedure" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="Family" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="FamilyMember" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="CodedTerm" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Quantity" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Subject" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Participant" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="AccessPolicy" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="BiospecimenCollection" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Aliquot" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Measurement" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Procedure" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="Family" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="FamilyMember" sheetId="18" state="visible" r:id="rId18"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -452,6 +456,307 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>subject_type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>organism_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>subject_assertion</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_access_policy</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"participant,non_participant,cell_line,animal_model,group,other"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>date_of_birth</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>date_of_birth_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>phenotypic_sex</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>phenotypic_sex_source_value</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>race</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>race_source_value</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>ethnicity</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>ethnicity_source_value</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>age_at_last_vital_status</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>vital_status</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>has_sample</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>has_assertion</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>subject_type</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>organism_type</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>subject_assertion</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>has_access_policy</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="6">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"exact,year_only,shifted,decade_only,other"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"female,male,unknown,intersex"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"american_indian_or_alaskan_native,asian,black_or_african_american,native_hawaiian_or_pacific_islander,white,other_race,unknown,asked_but_unknown"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"hispanic_or_latino,not_hispanic_or_latino,unknown,asked_but_unknown"</formula1>
+    </dataValidation>
+    <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"alive,dead,not_reported,unknown,unspecified"</formula1>
+    </dataValidation>
+    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"participant,non_participant,cell_line,animal_model,group,other"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>data_access_type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>access_policy_code</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>disease_limitation</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>website</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"open,registered,controlled,gsr_restricted,gsr_allowed"</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"gru,hmb,ds,irb,pub,col,npu,mds,gso,gsr"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>age_at_collection</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>method</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>site</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>spatial_qualifier</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>laterality</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -507,7 +812,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -563,7 +868,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -604,7 +909,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -663,7 +968,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -746,6 +1051,24 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -791,7 +1114,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -857,37 +1180,113 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>subject_type</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>organism_type</t>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>age_at_assertion</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>assertion</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>has_access_policy</t>
+          <t>value</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
+        <is>
+          <t>source_assertion</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>source_value</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>condition_type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>age_at_onset</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>age_at_resolution</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>age_at_assertion</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>assertion</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>source_assertion</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>source_value</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -896,261 +1295,40 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"participant,non_participant,cell_line,animal_model,group,other"</formula1>
+      <formula1>"phenotypic_feature,disease,comorbidity,histology,clinical_finding,ehr_billing_code"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:P1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>date_of_birth</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>date_of_birth_type</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>phenotypic_sex</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>phenotypic_sex_source_value</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>race</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>race_source_value</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>ethnicity</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>ethnicity_source_value</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>age_at_last_vital_status</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>vital_status</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>has_sample</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>has_assertion</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>subject_type</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>organism_type</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>has_access_policy</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="6">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"exact,year_only,shifted,decade_only,other"</formula1>
-    </dataValidation>
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"female,male,unknown,intersex"</formula1>
-    </dataValidation>
-    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"american_indian_or_alaskan_native,asian,black_or_african_american,native_hawaiian_or_pacific_islander,white,other_race,unknown,asked_but_unknown"</formula1>
-    </dataValidation>
-    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"hispanic_or_latino,not_hispanic_or_latino,unknown,asked_but_unknown"</formula1>
-    </dataValidation>
-    <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"alive,dead,not_reported,unknown,unspecified"</formula1>
-    </dataValidation>
-    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"participant,non_participant,cell_line,animal_model,group,other"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>condition_code</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>condition_source_value</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>condition_assertion</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>condition_type</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>age_at_assertion</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>age_at_onset</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>age_at_resolution</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
-    </dataValidation>
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"present,absent,unsure,unknown"</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"phenotypic_feature,disease,comorbidity,histology,clinical_finding,ehr_billing_code"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>data_access_type</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>access_policy_code</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>disease_limitation</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>website</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"open,registered,controlled,gsr_restricted,gsr_allowed"</formula1>
-    </dataValidation>
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"gru,hmb,ds,irb,pub,col,npu,mds,gso,gsr"</formula1>
-    </dataValidation>
-  </dataValidations>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>code</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>code_string</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1161,61 +1339,27 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>age_at_collection</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>method</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>site</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>spatial_qualifier</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>laterality</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="4">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
-    </dataValidation>
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
-    </dataValidation>
-    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
-    </dataValidation>
-  </dataValidations>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
:arrow_double_down: Generalize source data
Take source data out of the Subject Assertion into its own class. This may be removed entirely and rely on original data row references; the model still is effective in that setting.
</commit_message>
<xml_diff>
--- a/anvil/excel/anvil.xlsx
+++ b/anvil/excel/anvil.xlsx
@@ -14,13 +14,14 @@
     <sheet name="Subject" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Participant" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="SubjectAssertion" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="AccessPolicy" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="BiospecimenCollection" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Aliquot" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="Measurement" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="Procedure" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="Family" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="FamilyMember" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="SourceData" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="AccessPolicy" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="BiospecimenCollection" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Aliquot" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Measurement" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Procedure" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Family" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="FamilyMember" sheetId="15" state="visible" r:id="rId15"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -452,6 +453,71 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>age_at_collection</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>method</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>site</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>spatial_qualifier</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>laterality</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -507,7 +573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -563,7 +629,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -590,7 +656,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>age_at_observation</t>
+          <t>age_at_event</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -604,7 +670,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -663,7 +729,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1056,57 +1122,57 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>age_at_assertion</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>age_at_event</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>age_at_resolution</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>code</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>display</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>source_code</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>source_display</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>value_code</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>value_display</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>value_number</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>value_units</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>age_at_assertion</t>
-        </is>
-      </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>age_at_event</t>
+          <t>value_units_display</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>age_at_resolution</t>
+          <t>source_data</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
@@ -1136,6 +1202,72 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>code</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>display</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>value_code</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>value_display</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>value_number</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>value_units</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>value_units_display</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>has_access_policy</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1187,69 +1319,4 @@
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>age_at_collection</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>method</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>site</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>spatial_qualifier</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>laterality</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="4">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
-    </dataValidation>
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
-    </dataValidation>
-    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>